<commit_message>
see #284 can now display game screen on Firefox and Opera
</commit_message>
<xml_diff>
--- a/doc/image collage coordinates.xlsx
+++ b/doc/image collage coordinates.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -276,36 +276,18 @@
     <t>40x33</t>
   </si>
   <si>
-    <t>on_board_beach_animated_1.png</t>
-  </si>
-  <si>
     <t>68x92</t>
   </si>
   <si>
-    <t>on_board_beach_animated_2.png</t>
-  </si>
-  <si>
     <t>46x46</t>
   </si>
   <si>
-    <t>on_board_cave_animated_1.png</t>
-  </si>
-  <si>
     <t>52x92</t>
   </si>
   <si>
-    <t>on_board_cave_animated_2.png</t>
-  </si>
-  <si>
-    <t>on_board_forest_animated_1.png</t>
-  </si>
-  <si>
     <t>70x92</t>
   </si>
   <si>
-    <t>on_board_forest_animated_2.png</t>
-  </si>
-  <si>
     <t>466x115</t>
   </si>
   <si>
@@ -489,31 +471,49 @@
     <t>background_leaderboard_rank.png</t>
   </si>
   <si>
-    <t>talking_heads_base.png</t>
-  </si>
-  <si>
     <t>200x242</t>
   </si>
   <si>
-    <t>talking_heads_mouth.png</t>
-  </si>
-  <si>
     <t>120x123</t>
   </si>
   <si>
-    <t>talking_heads_eyes.png</t>
-  </si>
-  <si>
-    <t>right_head_eyes</t>
-  </si>
-  <si>
     <t>46x21</t>
   </si>
   <si>
-    <t>left_head_eyes</t>
-  </si>
-  <si>
     <t>37x21</t>
+  </si>
+  <si>
+    <t>game-beach-jump-strips.png</t>
+  </si>
+  <si>
+    <t>game-beach-rollover-strips.png</t>
+  </si>
+  <si>
+    <t>game-cave-jump-strips.png</t>
+  </si>
+  <si>
+    <t>game-cave-rollover-strips.png</t>
+  </si>
+  <si>
+    <t>game-forest-jump-strips.png</t>
+  </si>
+  <si>
+    <t>game-forest-rollover-strips.png</t>
+  </si>
+  <si>
+    <t>collage/heads-eyes-strip.png</t>
+  </si>
+  <si>
+    <t>heads-base.png</t>
+  </si>
+  <si>
+    <t>heads-mouth-strip.png</t>
+  </si>
+  <si>
+    <t>heads-right-eyes-strip.png</t>
+  </si>
+  <si>
+    <t>heads-left-eyes-strip.png</t>
   </si>
 </sst>
 </file>
@@ -850,11 +850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N120"/>
+  <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -1537,12 +1537,12 @@
         <v>92</v>
       </c>
       <c r="K60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -1557,12 +1557,12 @@
         <v>46</v>
       </c>
       <c r="K61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -1577,12 +1577,12 @@
         <v>92</v>
       </c>
       <c r="K62" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -1597,12 +1597,12 @@
         <v>46</v>
       </c>
       <c r="K63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -1617,12 +1617,12 @@
         <v>92</v>
       </c>
       <c r="K64" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -1637,12 +1637,12 @@
         <v>46</v>
       </c>
       <c r="K65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -1654,12 +1654,12 @@
         <v>58</v>
       </c>
       <c r="K67" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -1671,12 +1671,12 @@
         <v>122</v>
       </c>
       <c r="K68" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -1688,12 +1688,12 @@
         <v>33</v>
       </c>
       <c r="K69" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -1705,12 +1705,12 @@
         <v>18</v>
       </c>
       <c r="K70" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -1722,12 +1722,12 @@
         <v>30</v>
       </c>
       <c r="K71" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -1739,12 +1739,12 @@
         <v>46</v>
       </c>
       <c r="K72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -1759,12 +1759,12 @@
         <v>46</v>
       </c>
       <c r="K74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -1779,12 +1779,12 @@
         <v>46</v>
       </c>
       <c r="K75" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -1799,12 +1799,12 @@
         <v>46</v>
       </c>
       <c r="K76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -1819,17 +1819,17 @@
         <v>46</v>
       </c>
       <c r="K77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="D82" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -1838,12 +1838,12 @@
         <v>0</v>
       </c>
       <c r="K82" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="D83" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -1852,12 +1852,12 @@
         <v>29</v>
       </c>
       <c r="K83" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="D84" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -1866,12 +1866,12 @@
         <v>75</v>
       </c>
       <c r="K84" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="D85" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -1880,12 +1880,12 @@
         <v>117</v>
       </c>
       <c r="K85" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="D86" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -1894,12 +1894,12 @@
         <v>174</v>
       </c>
       <c r="K86" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:11">
       <c r="D87" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -1908,12 +1908,12 @@
         <v>201</v>
       </c>
       <c r="K87" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="D88" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -1922,12 +1922,12 @@
         <v>228</v>
       </c>
       <c r="K88" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="D89" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -1936,12 +1936,12 @@
         <v>269</v>
       </c>
       <c r="K89" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:11">
       <c r="D90" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -1950,12 +1950,12 @@
         <v>312</v>
       </c>
       <c r="K90" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:11">
       <c r="D91" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -1964,12 +1964,12 @@
         <v>367</v>
       </c>
       <c r="K91" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="D92" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -1978,17 +1978,17 @@
         <v>397</v>
       </c>
       <c r="K92" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:11">
       <c r="D96" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -1997,12 +1997,12 @@
         <v>0</v>
       </c>
       <c r="K96" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="D97" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G97">
         <v>49</v>
@@ -2011,12 +2011,12 @@
         <v>0</v>
       </c>
       <c r="K97" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:11">
       <c r="D98" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G98">
         <v>98</v>
@@ -2025,12 +2025,12 @@
         <v>0</v>
       </c>
       <c r="K98" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="D99" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G99">
         <v>131</v>
@@ -2039,12 +2039,12 @@
         <v>0</v>
       </c>
       <c r="K99" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="D100" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G100">
         <v>164</v>
@@ -2053,12 +2053,12 @@
         <v>0</v>
       </c>
       <c r="K100" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="D101" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G101">
         <v>197</v>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="K101" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -2081,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="K102" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="K103" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="K104" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -2123,68 +2123,68 @@
         <v>0</v>
       </c>
       <c r="K105" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K108" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="K109" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K110" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K111" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K112" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K113" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K115" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -2196,17 +2196,17 @@
         <v>60</v>
       </c>
       <c r="K116" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:12">
       <c r="D119" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -2218,12 +2218,12 @@
         <v>46</v>
       </c>
       <c r="K119" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="D120" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -2235,7 +2235,45 @@
         <v>37</v>
       </c>
       <c r="K120" t="s">
-        <v>165</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122">
+        <v>0</v>
+      </c>
+      <c r="B122">
+        <v>46</v>
+      </c>
+      <c r="C122">
+        <v>92</v>
+      </c>
+      <c r="D122">
+        <v>138</v>
+      </c>
+      <c r="E122">
+        <v>184</v>
+      </c>
+      <c r="F122">
+        <v>230</v>
+      </c>
+      <c r="G122">
+        <v>276</v>
+      </c>
+      <c r="H122">
+        <v>322</v>
+      </c>
+      <c r="I122">
+        <v>368</v>
+      </c>
+      <c r="J122">
+        <v>414</v>
+      </c>
+      <c r="K122">
+        <v>460</v>
+      </c>
+      <c r="L122">
+        <v>506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>